<commit_message>
Viaticos_q_estimacion de esfuerzo actualizado
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/1. Estimacion/Viaticos_q_Estimación_Esfuerzo.xlsx
+++ b/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/1. Estimacion/Viaticos_q_Estimación_Esfuerzo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Proyectos\Activos\Viaticos_q\2. Estimacion y planeacion\1. Plantillas estimacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Proyectos\Activos\Viaticos_q\2. Estimacion y planeacion\1. Estimacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,6 @@
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="AvanceEstFecha">'[1]Métricas Base Workflow'!$F$95</definedName>
@@ -2662,63 +2661,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instrucciones"/>
-      <sheetName val="Factor de complejidad Téc y Amb"/>
-      <sheetName val="Estimación de Tamaño UCP"/>
-      <sheetName val="Estimación de Esfuerzo"/>
-      <sheetName val="Recursos"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="5">
-          <cell r="E5">
-            <v>59.853275767543863</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6">
-            <v>51.617173793859649</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7">
-            <v>51.617173793859649</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8">
-            <v>59.853275767543863</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>31.977576754385964</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>31.977576754385964</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>59.853275767543863</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B7:C10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="2">
@@ -3937,7 +3879,7 @@
   <dimension ref="B2:K42"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4557,7 +4499,7 @@
         <v>65</v>
       </c>
       <c r="G42" s="216">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H42" s="217"/>
     </row>
@@ -5170,8 +5112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5383,7 +5325,7 @@
       <c r="J9" s="238"/>
       <c r="K9" s="203">
         <f>SUM(K10:K15)</f>
-        <v>1496.8980400219298</v>
+        <v>1826.9240816885965</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -5407,12 +5349,12 @@
         <v>86</v>
       </c>
       <c r="J10" s="91">
-        <f>IF(I10="Líder de proyecto",[5]Recursos!E$5,(IF(I10="Analista",[5]Recursos!E$6,(IF(I10="Diseñador",[5]Recursos!#REF!,(IF(I10="Tester",[5]Recursos!E$7,(IF(I10="Desarrollador",[5]Recursos!E$8,(IF(I10="Arquitecto",[5]Recursos!E$12,(IF(I10="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I10="Líder de proyecto",Recursos!E$5,(IF(I10="Analista",Recursos!E$6,(IF(I10="Diseñador",Recursos!#REF!,(IF(I10="Tester",Recursos!E$7,(IF(I10="Desarrollador",Recursos!E$8,(IF(I10="Arquitecto",Recursos!E$12,(IF(I10="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K10" s="117">
         <f t="shared" ref="K10:K15" si="0">F10*J10*G10</f>
-        <v>361.32021655701755</v>
+        <v>440.98167489035086</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -5436,12 +5378,12 @@
         <v>86</v>
       </c>
       <c r="J11" s="91">
-        <f>IF(I11="Líder de proyecto",[5]Recursos!E$5,(IF(I11="Analista",[5]Recursos!E$6,(IF(I11="Diseñador",[5]Recursos!#REF!,(IF(I11="Tester",[5]Recursos!E$7,(IF(I11="Desarrollador",[5]Recursos!E$8,(IF(I11="Arquitecto",[5]Recursos!E$12,(IF(I11="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I11="Líder de proyecto",Recursos!E$5,(IF(I11="Analista",Recursos!E$6,(IF(I11="Diseñador",Recursos!#REF!,(IF(I11="Tester",Recursos!E$7,(IF(I11="Desarrollador",Recursos!E$8,(IF(I11="Arquitecto",Recursos!E$12,(IF(I11="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K11" s="117">
         <f t="shared" si="0"/>
-        <v>154.85152138157895</v>
+        <v>188.99214638157895</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -5465,12 +5407,12 @@
         <v>86</v>
       </c>
       <c r="J12" s="91">
-        <f>IF(I12="Líder de proyecto",[5]Recursos!E$5,(IF(I12="Analista",[5]Recursos!E$6,(IF(I12="Diseñador",[5]Recursos!#REF!,(IF(I12="Tester",[5]Recursos!E$7,(IF(I12="Desarrollador",[5]Recursos!E$8,(IF(I12="Arquitecto",[5]Recursos!E$12,(IF(I12="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I12="Líder de proyecto",Recursos!E$5,(IF(I12="Analista",Recursos!E$6,(IF(I12="Diseñador",Recursos!#REF!,(IF(I12="Tester",Recursos!E$7,(IF(I12="Desarrollador",Recursos!E$8,(IF(I12="Arquitecto",Recursos!E$12,(IF(I12="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K12" s="117">
         <f t="shared" si="0"/>
-        <v>103.2343475877193</v>
+        <v>125.99476425438596</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -5494,12 +5436,12 @@
         <v>86</v>
       </c>
       <c r="J13" s="91">
-        <f>IF(I13="Líder de proyecto",[5]Recursos!E$5,(IF(I13="Analista",[5]Recursos!E$6,(IF(I13="Diseñador",[5]Recursos!#REF!,(IF(I13="Tester",[5]Recursos!E$7,(IF(I13="Desarrollador",[5]Recursos!E$8,(IF(I13="Arquitecto",[5]Recursos!E$12,(IF(I13="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I13="Líder de proyecto",Recursos!E$5,(IF(I13="Analista",Recursos!E$6,(IF(I13="Diseñador",Recursos!#REF!,(IF(I13="Tester",Recursos!E$7,(IF(I13="Desarrollador",Recursos!E$8,(IF(I13="Arquitecto",Recursos!E$12,(IF(I13="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K13" s="117">
         <f t="shared" si="0"/>
-        <v>619.40608552631579</v>
+        <v>755.96858552631579</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -5523,12 +5465,12 @@
         <v>86</v>
       </c>
       <c r="J14" s="91">
-        <f>IF(I14="Líder de proyecto",[5]Recursos!E$5,(IF(I14="Analista",[5]Recursos!E$6,(IF(I14="Diseñador",[5]Recursos!#REF!,(IF(I14="Tester",[5]Recursos!E$7,(IF(I14="Desarrollador",[5]Recursos!E$8,(IF(I14="Arquitecto",[5]Recursos!E$12,(IF(I14="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I14="Líder de proyecto",Recursos!E$5,(IF(I14="Analista",Recursos!E$6,(IF(I14="Diseñador",Recursos!#REF!,(IF(I14="Tester",Recursos!E$7,(IF(I14="Desarrollador",Recursos!E$8,(IF(I14="Arquitecto",Recursos!E$12,(IF(I14="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K14" s="117">
         <f t="shared" si="0"/>
-        <v>51.617173793859649</v>
+        <v>62.997382127192978</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -5552,12 +5494,12 @@
         <v>86</v>
       </c>
       <c r="J15" s="91">
-        <f>IF(I15="Líder de proyecto",[5]Recursos!E$5,(IF(I15="Analista",[5]Recursos!E$6,(IF(I15="Diseñador",[5]Recursos!#REF!,(IF(I15="Tester",[5]Recursos!E$7,(IF(I15="Desarrollador",[5]Recursos!E$8,(IF(I15="Arquitecto",[5]Recursos!E$12,(IF(I15="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I15="Líder de proyecto",Recursos!E$5,(IF(I15="Analista",Recursos!E$6,(IF(I15="Diseñador",Recursos!#REF!,(IF(I15="Tester",Recursos!E$7,(IF(I15="Desarrollador",Recursos!E$8,(IF(I15="Arquitecto",Recursos!E$12,(IF(I15="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K15" s="117">
         <f t="shared" si="0"/>
-        <v>206.4686951754386</v>
+        <v>251.98952850877191</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -5586,7 +5528,7 @@
       </c>
       <c r="K16" s="203">
         <f>SUM(K17+K25)</f>
-        <v>2745.0145833333336</v>
+        <v>3268.5041666666666</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5610,7 +5552,7 @@
       </c>
       <c r="K17" s="204">
         <f>SUM(K18:K24)</f>
-        <v>1128.9761376096494</v>
+        <v>1345.2000959429824</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5634,12 +5576,12 @@
         <v>85</v>
       </c>
       <c r="J18" s="91">
-        <f>IF(I18="Líder de proyecto",[5]Recursos!E$5,(IF(I18="Analista",[5]Recursos!E$6,(IF(I18="Diseñador",[5]Recursos!#REF!,(IF(I18="Tester",[5]Recursos!E$7,(IF(I18="Desarrollador",[5]Recursos!E$8,(IF(I18="Arquitecto",[5]Recursos!E$12,(IF(I18="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I18="Líder de proyecto",Recursos!E$5,(IF(I18="Analista",Recursos!E$6,(IF(I18="Diseñador",Recursos!#REF!,(IF(I18="Tester",Recursos!E$7,(IF(I18="Desarrollador",Recursos!E$8,(IF(I18="Arquitecto",Recursos!E$12,(IF(I18="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K18" s="117">
         <f>F18*J18*G18</f>
-        <v>119.70655153508773</v>
+        <v>142.46696820175438</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5663,12 +5605,12 @@
         <v>85</v>
       </c>
       <c r="J19" s="91">
-        <f>IF(I19="Líder de proyecto",[5]Recursos!E$5,(IF(I19="Analista",[5]Recursos!E$6,(IF(I19="Diseñador",[5]Recursos!#REF!,(IF(I19="Tester",[5]Recursos!E$7,(IF(I19="Desarrollador",[5]Recursos!E$8,(IF(I19="Arquitecto",[5]Recursos!E$12,(IF(I19="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I19="Líder de proyecto",Recursos!E$5,(IF(I19="Analista",Recursos!E$6,(IF(I19="Diseñador",Recursos!#REF!,(IF(I19="Tester",Recursos!E$7,(IF(I19="Desarrollador",Recursos!E$8,(IF(I19="Arquitecto",Recursos!E$12,(IF(I19="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K19" s="117">
         <f>F19*J19*G19</f>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5692,12 +5634,12 @@
         <v>85</v>
       </c>
       <c r="J20" s="91">
-        <f>IF(I20="Líder de proyecto",[5]Recursos!E$5,(IF(I20="Analista",[5]Recursos!E$6,(IF(I20="Diseñador",[5]Recursos!#REF!,(IF(I20="Tester",[5]Recursos!E$7,(IF(I20="Desarrollador",[5]Recursos!E$8,(IF(I20="Arquitecto",[5]Recursos!E$12,(IF(I20="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I20="Líder de proyecto",Recursos!E$5,(IF(I20="Analista",Recursos!E$6,(IF(I20="Diseñador",Recursos!#REF!,(IF(I20="Tester",Recursos!E$7,(IF(I20="Desarrollador",Recursos!E$8,(IF(I20="Arquitecto",Recursos!E$12,(IF(I20="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K20" s="117">
         <f t="shared" ref="K20:K22" si="1">F20*J20*G20</f>
-        <v>359.11965460526318</v>
+        <v>427.40090460526312</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5721,12 +5663,12 @@
         <v>86</v>
       </c>
       <c r="J21" s="91">
-        <f>IF(I21="Líder de proyecto",[5]Recursos!E$5,(IF(I21="Analista",[5]Recursos!E$6,(IF(I21="Diseñador",[5]Recursos!#REF!,(IF(I21="Tester",[5]Recursos!E$7,(IF(I21="Desarrollador",[5]Recursos!E$8,(IF(I21="Arquitecto",[5]Recursos!E$12,(IF(I21="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I21="Líder de proyecto",Recursos!E$5,(IF(I21="Analista",Recursos!E$6,(IF(I21="Diseñador",Recursos!#REF!,(IF(I21="Tester",Recursos!E$7,(IF(I21="Desarrollador",Recursos!E$8,(IF(I21="Arquitecto",Recursos!E$12,(IF(I21="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K21" s="117">
         <f t="shared" si="1"/>
-        <v>51.617173793859649</v>
+        <v>62.997382127192978</v>
       </c>
       <c r="N21" s="135"/>
     </row>
@@ -5751,12 +5693,12 @@
         <v>85</v>
       </c>
       <c r="J22" s="91">
-        <f>IF(I22="Líder de proyecto",[5]Recursos!E$5,(IF(I22="Analista",[5]Recursos!E$6,(IF(I22="Diseñador",[5]Recursos!#REF!,(IF(I22="Tester",[5]Recursos!E$7,(IF(I22="Desarrollador",[5]Recursos!E$8,(IF(I22="Arquitecto",[5]Recursos!E$12,(IF(I22="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I22="Líder de proyecto",Recursos!E$5,(IF(I22="Analista",Recursos!E$6,(IF(I22="Diseñador",Recursos!#REF!,(IF(I22="Tester",Recursos!E$7,(IF(I22="Desarrollador",Recursos!E$8,(IF(I22="Arquitecto",Recursos!E$12,(IF(I22="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K22" s="117">
         <f t="shared" si="1"/>
-        <v>59.853275767543863</v>
+        <v>71.233484100877192</v>
       </c>
       <c r="N22" s="135"/>
     </row>
@@ -5781,12 +5723,12 @@
         <v>85</v>
       </c>
       <c r="J23" s="91">
-        <f>IF(I23="Líder de proyecto",[5]Recursos!E$5,(IF(I23="Analista",[5]Recursos!E$6,(IF(I23="Diseñador",[5]Recursos!#REF!,(IF(I23="Tester",[5]Recursos!E$7,(IF(I23="Desarrollador",[5]Recursos!E$8,(IF(I23="Arquitecto",[5]Recursos!E$12,(IF(I23="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I23="Líder de proyecto",Recursos!E$5,(IF(I23="Analista",Recursos!E$6,(IF(I23="Diseñador",Recursos!#REF!,(IF(I23="Tester",Recursos!E$7,(IF(I23="Desarrollador",Recursos!E$8,(IF(I23="Arquitecto",Recursos!E$12,(IF(I23="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K23" s="118">
         <f>F23*J23*G23</f>
-        <v>59.853275767543863</v>
+        <v>71.233484100877192</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5810,12 +5752,12 @@
         <v>85</v>
       </c>
       <c r="J24" s="91">
-        <f>IF(I24="Líder de proyecto",[5]Recursos!E$5,(IF(I24="Analista",[5]Recursos!E$6,(IF(I24="Diseñador",[5]Recursos!#REF!,(IF(I24="Tester",[5]Recursos!E$7,(IF(I24="Desarrollador",[5]Recursos!E$8,(IF(I24="Arquitecto",[5]Recursos!E$12,(IF(I24="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I24="Líder de proyecto",Recursos!E$5,(IF(I24="Analista",Recursos!E$6,(IF(I24="Diseñador",Recursos!#REF!,(IF(I24="Tester",Recursos!E$7,(IF(I24="Desarrollador",Recursos!E$8,(IF(I24="Arquitecto",Recursos!E$12,(IF(I24="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K24" s="118">
         <f>F24*J24*G24</f>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5839,7 +5781,7 @@
       </c>
       <c r="K25" s="204">
         <f>SUM(K26:K29)</f>
-        <v>1616.0384457236844</v>
+        <v>1923.3040707236839</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5862,12 +5804,12 @@
         <v>85</v>
       </c>
       <c r="J26" s="91">
-        <f>IF(I26="Líder de proyecto",[5]Recursos!E$5,(IF(I26="Analista",[5]Recursos!E$6,(IF(I26="Diseñador",[5]Recursos!#REF!,(IF(I26="Tester",[5]Recursos!E$7,(IF(I26="Desarrollador",[5]Recursos!E$8,(IF(I26="Arquitecto",[5]Recursos!E$12,(IF(I26="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I26="Líder de proyecto",Recursos!E$5,(IF(I26="Analista",Recursos!E$6,(IF(I26="Diseñador",Recursos!#REF!,(IF(I26="Tester",Recursos!E$7,(IF(I26="Desarrollador",Recursos!E$8,(IF(I26="Arquitecto",Recursos!E$12,(IF(I26="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K26" s="117">
         <f t="shared" ref="K26:K29" si="2">F26*J26*G26</f>
-        <v>658.38603344298247</v>
+        <v>783.56832510964909</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5891,12 +5833,12 @@
         <v>85</v>
       </c>
       <c r="J27" s="91">
-        <f>IF(I27="Líder de proyecto",[5]Recursos!E$5,(IF(I27="Analista",[5]Recursos!E$6,(IF(I27="Diseñador",[5]Recursos!#REF!,(IF(I27="Tester",[5]Recursos!E$7,(IF(I27="Desarrollador",[5]Recursos!E$8,(IF(I27="Arquitecto",[5]Recursos!E$12,(IF(I27="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I27="Líder de proyecto",Recursos!E$5,(IF(I27="Analista",Recursos!E$6,(IF(I27="Diseñador",Recursos!#REF!,(IF(I27="Tester",Recursos!E$7,(IF(I27="Desarrollador",Recursos!E$8,(IF(I27="Arquitecto",Recursos!E$12,(IF(I27="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K27" s="117">
         <f t="shared" si="2"/>
-        <v>778.09258497807025</v>
+        <v>926.03529331140351</v>
       </c>
     </row>
     <row r="28" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5920,12 +5862,12 @@
         <v>85</v>
       </c>
       <c r="J28" s="91">
-        <f>IF(I28="Líder de proyecto",[5]Recursos!E$5,(IF(I28="Analista",[5]Recursos!E$6,(IF(I28="Diseñador",[5]Recursos!#REF!,(IF(I28="Tester",[5]Recursos!E$7,(IF(I28="Desarrollador",[5]Recursos!E$8,(IF(I28="Arquitecto",[5]Recursos!E$12,(IF(I28="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I28="Líder de proyecto",Recursos!E$5,(IF(I28="Analista",Recursos!E$6,(IF(I28="Diseñador",Recursos!#REF!,(IF(I28="Tester",Recursos!E$7,(IF(I28="Desarrollador",Recursos!E$8,(IF(I28="Arquitecto",Recursos!E$12,(IF(I28="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K28" s="117">
         <f t="shared" si="2"/>
-        <v>59.853275767543863</v>
+        <v>71.233484100877192</v>
       </c>
     </row>
     <row r="29" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5949,12 +5891,12 @@
         <v>85</v>
       </c>
       <c r="J29" s="91">
-        <f>IF(I29="Líder de proyecto",[5]Recursos!E$5,(IF(I29="Analista",[5]Recursos!E$6,(IF(I29="Diseñador",[5]Recursos!#REF!,(IF(I29="Tester",[5]Recursos!E$7,(IF(I29="Desarrollador",[5]Recursos!E$8,(IF(I29="Arquitecto",[5]Recursos!E$12,(IF(I29="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I29="Líder de proyecto",Recursos!E$5,(IF(I29="Analista",Recursos!E$6,(IF(I29="Diseñador",Recursos!#REF!,(IF(I29="Tester",Recursos!E$7,(IF(I29="Desarrollador",Recursos!E$8,(IF(I29="Arquitecto",Recursos!E$12,(IF(I29="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K29" s="117">
         <f t="shared" si="2"/>
-        <v>119.70655153508773</v>
+        <v>142.46696820175438</v>
       </c>
     </row>
     <row r="30" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5983,7 +5925,7 @@
       </c>
       <c r="K30" s="203">
         <f>SUM(K38+K36+K44+K31)</f>
-        <v>6307.667845394737</v>
+        <v>7536.7303453947361</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -6012,7 +5954,7 @@
       </c>
       <c r="K31" s="205">
         <f>SUM(K32:K35)</f>
-        <v>778.09258497807014</v>
+        <v>926.03529331140351</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -6036,12 +5978,12 @@
         <v>155</v>
       </c>
       <c r="J32" s="91">
-        <f>IF(I32="Líder de proyecto",[5]Recursos!E$5,(IF(I32="Analista",[5]Recursos!E$6,(IF(I32="Diseñador",[5]Recursos!#REF!,(IF(I32="Tester",[5]Recursos!E$7,(IF(I32="Desarrollador",[5]Recursos!E$8,(IF(I32="Arquitecto",[5]Recursos!E$12,(IF(I32="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I32="Líder de proyecto",Recursos!E$5,(IF(I32="Analista",Recursos!E$6,(IF(I32="Diseñador",Recursos!#REF!,(IF(I32="Tester",Recursos!E$7,(IF(I32="Desarrollador",Recursos!E$8,(IF(I32="Arquitecto",Recursos!E$12,(IF(I32="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K32" s="117">
         <f>F32*J32*G32</f>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6065,12 +6007,12 @@
         <v>155</v>
       </c>
       <c r="J33" s="91">
-        <f>IF(I33="Líder de proyecto",[5]Recursos!E$5,(IF(I33="Analista",[5]Recursos!E$6,(IF(I33="Diseñador",[5]Recursos!#REF!,(IF(I33="Tester",[5]Recursos!E$7,(IF(I33="Desarrollador",[5]Recursos!E$8,(IF(I33="Arquitecto",[5]Recursos!E$12,(IF(I33="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I33="Líder de proyecto",Recursos!E$5,(IF(I33="Analista",Recursos!E$6,(IF(I33="Diseñador",Recursos!#REF!,(IF(I33="Tester",Recursos!E$7,(IF(I33="Desarrollador",Recursos!E$8,(IF(I33="Arquitecto",Recursos!E$12,(IF(I33="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K33" s="117">
         <f t="shared" ref="K33:K35" si="3">F33*J33*G33</f>
-        <v>179.55982730263159</v>
+        <v>213.70045230263156</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6094,12 +6036,12 @@
         <v>155</v>
       </c>
       <c r="J34" s="91">
-        <f>IF(I34="Líder de proyecto",[5]Recursos!E$5,(IF(I34="Analista",[5]Recursos!E$6,(IF(I34="Diseñador",[5]Recursos!#REF!,(IF(I34="Tester",[5]Recursos!E$7,(IF(I34="Desarrollador",[5]Recursos!E$8,(IF(I34="Arquitecto",[5]Recursos!E$12,(IF(I34="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I34="Líder de proyecto",Recursos!E$5,(IF(I34="Analista",Recursos!E$6,(IF(I34="Diseñador",Recursos!#REF!,(IF(I34="Tester",Recursos!E$7,(IF(I34="Desarrollador",Recursos!E$8,(IF(I34="Arquitecto",Recursos!E$12,(IF(I34="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K34" s="117">
         <f t="shared" si="3"/>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6123,12 +6065,12 @@
         <v>155</v>
       </c>
       <c r="J35" s="91">
-        <f>IF(I35="Líder de proyecto",[5]Recursos!E$5,(IF(I35="Analista",[5]Recursos!E$6,(IF(I35="Diseñador",[5]Recursos!#REF!,(IF(I35="Tester",[5]Recursos!E$7,(IF(I35="Desarrollador",[5]Recursos!E$8,(IF(I35="Arquitecto",[5]Recursos!E$12,(IF(I35="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I35="Líder de proyecto",Recursos!E$5,(IF(I35="Analista",Recursos!E$6,(IF(I35="Diseñador",Recursos!#REF!,(IF(I35="Tester",Recursos!E$7,(IF(I35="Desarrollador",Recursos!E$8,(IF(I35="Arquitecto",Recursos!E$12,(IF(I35="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K35" s="117">
         <f t="shared" si="3"/>
-        <v>119.70655153508773</v>
+        <v>142.46696820175438</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6157,7 +6099,7 @@
       </c>
       <c r="K36" s="205">
         <f>SUM(K37:K37)</f>
-        <v>3890.4629248903511</v>
+        <v>4630.1764665570172</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6181,12 +6123,12 @@
         <v>169</v>
       </c>
       <c r="J37" s="91">
-        <f>IF(I37="Líder de proyecto",[5]Recursos!E$5,(IF(I37="Analista",[5]Recursos!E$6,(IF(I37="Diseñador",[5]Recursos!#REF!,(IF(I37="Tester",[5]Recursos!E$7,(IF(I37="Desarrollador",[5]Recursos!E$8,(IF(I37="Arquitecto",[5]Recursos!E$12,(IF(I37="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I37="Líder de proyecto",Recursos!E$5,(IF(I37="Analista",Recursos!E$6,(IF(I37="Diseñador",Recursos!#REF!,(IF(I37="Tester",Recursos!E$7,(IF(I37="Desarrollador",Recursos!E$8,(IF(I37="Arquitecto",Recursos!E$12,(IF(I37="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K37" s="118">
         <f>F37*J37*G37</f>
-        <v>3890.4629248903511</v>
+        <v>4630.1764665570172</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6215,7 +6157,7 @@
       </c>
       <c r="K38" s="205">
         <f>SUM(K39:K43)</f>
-        <v>747.34873903508765</v>
+        <v>906.67165570175428</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6239,12 +6181,12 @@
         <v>87</v>
       </c>
       <c r="J39" s="91">
-        <f>IF(I39="Líder de proyecto",[5]Recursos!E$5,(IF(I39="Analista",[5]Recursos!E$6,(IF(I39="Diseñador",[5]Recursos!#REF!,(IF(I39="Tester",[5]Recursos!E$7,(IF(I39="Desarrollador",[5]Recursos!E$8,(IF(I39="Arquitecto",[5]Recursos!E$12,(IF(I39="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I39="Líder de proyecto",Recursos!E$5,(IF(I39="Analista",Recursos!E$6,(IF(I39="Diseñador",Recursos!#REF!,(IF(I39="Tester",Recursos!E$7,(IF(I39="Desarrollador",Recursos!E$8,(IF(I39="Arquitecto",Recursos!E$12,(IF(I39="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K39" s="117">
         <f>F39*J39*G39</f>
-        <v>154.85152138157895</v>
+        <v>188.99214638157895</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6268,12 +6210,12 @@
         <v>87</v>
       </c>
       <c r="J40" s="91">
-        <f>IF(I40="Líder de proyecto",[5]Recursos!E$5,(IF(I40="Analista",[5]Recursos!E$6,(IF(I40="Diseñador",[5]Recursos!#REF!,(IF(I40="Tester",[5]Recursos!E$7,(IF(I40="Desarrollador",[5]Recursos!E$8,(IF(I40="Arquitecto",[5]Recursos!E$12,(IF(I40="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I40="Líder de proyecto",Recursos!E$5,(IF(I40="Analista",Recursos!E$6,(IF(I40="Diseñador",Recursos!#REF!,(IF(I40="Tester",Recursos!E$7,(IF(I40="Desarrollador",Recursos!E$8,(IF(I40="Arquitecto",Recursos!E$12,(IF(I40="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K40" s="117">
         <f>F40*J40*G40</f>
-        <v>154.85152138157895</v>
+        <v>188.99214638157895</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6297,12 +6239,12 @@
         <v>169</v>
       </c>
       <c r="J41" s="91">
-        <f>IF(I41="Líder de proyecto",[5]Recursos!E$5,(IF(I41="Analista",[5]Recursos!E$6,(IF(I41="Diseñador",[5]Recursos!#REF!,(IF(I41="Tester",[5]Recursos!E$7,(IF(I41="Desarrollador",[5]Recursos!E$8,(IF(I41="Arquitecto",[5]Recursos!E$12,(IF(I41="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I41="Líder de proyecto",Recursos!E$5,(IF(I41="Analista",Recursos!E$6,(IF(I41="Diseñador",Recursos!#REF!,(IF(I41="Tester",Recursos!E$7,(IF(I41="Desarrollador",Recursos!E$8,(IF(I41="Arquitecto",Recursos!E$12,(IF(I41="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K41" s="117">
         <f>F41*J41*G41</f>
-        <v>179.55982730263159</v>
+        <v>213.70045230263156</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6326,12 +6268,12 @@
         <v>87</v>
       </c>
       <c r="J42" s="91">
-        <f>IF(I42="Líder de proyecto",[5]Recursos!E$5,(IF(I42="Analista",[5]Recursos!E$6,(IF(I42="Diseñador",[5]Recursos!#REF!,(IF(I42="Tester",[5]Recursos!E$7,(IF(I42="Desarrollador",[5]Recursos!E$8,(IF(I42="Arquitecto",[5]Recursos!E$12,(IF(I42="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I42="Líder de proyecto",Recursos!E$5,(IF(I42="Analista",Recursos!E$6,(IF(I42="Diseñador",Recursos!#REF!,(IF(I42="Tester",Recursos!E$7,(IF(I42="Desarrollador",Recursos!E$8,(IF(I42="Arquitecto",Recursos!E$12,(IF(I42="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K42" s="117">
         <f>F42*J42*G42</f>
-        <v>206.4686951754386</v>
+        <v>251.98952850877191</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6356,12 +6298,12 @@
         <v>87</v>
       </c>
       <c r="J43" s="91">
-        <f>IF(I43="Líder de proyecto",[5]Recursos!E$5,(IF(I43="Analista",[5]Recursos!E$6,(IF(I43="Diseñador",[5]Recursos!#REF!,(IF(I43="Tester",[5]Recursos!E$7,(IF(I43="Desarrollador",[5]Recursos!E$8,(IF(I43="Arquitecto",[5]Recursos!E$12,(IF(I43="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I43="Líder de proyecto",Recursos!E$5,(IF(I43="Analista",Recursos!E$6,(IF(I43="Diseñador",Recursos!#REF!,(IF(I43="Tester",Recursos!E$7,(IF(I43="Desarrollador",Recursos!E$8,(IF(I43="Arquitecto",Recursos!E$12,(IF(I43="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K43" s="117">
         <f>F43*J43*G43</f>
-        <v>51.617173793859649</v>
+        <v>62.997382127192978</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6390,7 +6332,7 @@
       </c>
       <c r="K44" s="205">
         <f>SUM(K45:K46)</f>
-        <v>891.7635964912281</v>
+        <v>1073.8469298245614</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6413,12 +6355,12 @@
         <v>155</v>
       </c>
       <c r="J45" s="91">
-        <f>IF(I45="Líder de proyecto",[5]Recursos!E$5,(IF(I45="Analista",[5]Recursos!E$6,(IF(I45="Diseñador",[5]Recursos!#REF!,(IF(I45="Tester",[5]Recursos!E$7,(IF(I45="Desarrollador",[5]Recursos!E$8,(IF(I45="Arquitecto",[5]Recursos!E$12,(IF(I45="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I45="Líder de proyecto",Recursos!E$5,(IF(I45="Analista",Recursos!E$6,(IF(I45="Diseñador",Recursos!#REF!,(IF(I45="Tester",Recursos!E$7,(IF(I45="Desarrollador",Recursos!E$8,(IF(I45="Arquitecto",Recursos!E$12,(IF(I45="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K45" s="117">
         <f>F45*J45*G45</f>
-        <v>478.82620614035091</v>
+        <v>569.86787280701753</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6441,12 +6383,12 @@
         <v>86</v>
       </c>
       <c r="J46" s="91">
-        <f>IF(I46="Líder de proyecto",[5]Recursos!E$5,(IF(I46="Analista",[5]Recursos!E$6,(IF(I46="Diseñador",[5]Recursos!#REF!,(IF(I46="Tester",[5]Recursos!E$7,(IF(I46="Desarrollador",[5]Recursos!E$8,(IF(I46="Arquitecto",[5]Recursos!E$12,(IF(I46="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>51.617173793859649</v>
+        <f>IF(I46="Líder de proyecto",Recursos!E$5,(IF(I46="Analista",Recursos!E$6,(IF(I46="Diseñador",Recursos!#REF!,(IF(I46="Tester",Recursos!E$7,(IF(I46="Desarrollador",Recursos!E$8,(IF(I46="Arquitecto",Recursos!E$12,(IF(I46="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>62.997382127192978</v>
       </c>
       <c r="K46" s="117">
         <f>F46*J46*G46</f>
-        <v>412.93739035087719</v>
+        <v>503.97905701754382</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6475,7 +6417,7 @@
       </c>
       <c r="K47" s="203">
         <f>SUM(K48:K49)</f>
-        <v>478.82620614035091</v>
+        <v>569.86787280701753</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6500,12 +6442,12 @@
         <v>85</v>
       </c>
       <c r="J48" s="91">
-        <f>IF(I48="Líder de proyecto",[5]Recursos!E$5,(IF(I48="Analista",[5]Recursos!E$6,(IF(I48="Diseñador",[5]Recursos!#REF!,(IF(I48="Tester",[5]Recursos!E$7,(IF(I48="Desarrollador",[5]Recursos!E$8,(IF(I48="Arquitecto",[5]Recursos!E$12,(IF(I48="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I48="Líder de proyecto",Recursos!E$5,(IF(I48="Analista",Recursos!E$6,(IF(I48="Diseñador",Recursos!#REF!,(IF(I48="Tester",Recursos!E$7,(IF(I48="Desarrollador",Recursos!E$8,(IF(I48="Arquitecto",Recursos!E$12,(IF(I48="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K48" s="117">
         <f>F48*J48*G48</f>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -6528,12 +6470,12 @@
         <v>85</v>
       </c>
       <c r="J49" s="91">
-        <f>IF(I49="Líder de proyecto",[5]Recursos!E$5,(IF(I49="Analista",[5]Recursos!E$6,(IF(I49="Diseñador",[5]Recursos!#REF!,(IF(I49="Tester",[5]Recursos!E$7,(IF(I49="Desarrollador",[5]Recursos!E$8,(IF(I49="Arquitecto",[5]Recursos!E$12,(IF(I49="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I49="Líder de proyecto",Recursos!E$5,(IF(I49="Analista",Recursos!E$6,(IF(I49="Diseñador",Recursos!#REF!,(IF(I49="Tester",Recursos!E$7,(IF(I49="Desarrollador",Recursos!E$8,(IF(I49="Arquitecto",Recursos!E$12,(IF(I49="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K49" s="117">
         <f>F49*J49*G49</f>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -6562,7 +6504,7 @@
       </c>
       <c r="K50" s="203">
         <f>SUM(K51:K54)</f>
-        <v>1598.0413925438597</v>
+        <v>2087.3903508771932</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -6586,12 +6528,12 @@
         <v>171</v>
       </c>
       <c r="J51" s="91">
-        <f>IF(I51="Líder de proyecto",[5]Recursos!E$5,(IF(I51="Analista",[5]Recursos!E$6,(IF(I51="Administrador de la configuración",[5]Recursos!E$11,(IF(I51="Tester",[5]Recursos!E$7,(IF(I51="Desarrollador",[5]Recursos!E$8,(IF(I51="Arquitecto",[5]Recursos!E$12,(IF(I51="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>31.977576754385964</v>
+        <f>IF(I51="Líder de proyecto",Recursos!E$5,(IF(I51="Analista",Recursos!E$6,(IF(I51="Administrador de la configuración",Recursos!E$11,(IF(I51="Tester",Recursos!E$7,(IF(I51="Desarrollador",Recursos!E$8,(IF(I51="Arquitecto",Recursos!E$12,(IF(I51="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>43.3577850877193</v>
       </c>
       <c r="K51" s="128">
         <f>F51*J51*G51</f>
-        <v>415.70849780701752</v>
+        <v>563.65120614035095</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -6617,12 +6559,12 @@
         <v>170</v>
       </c>
       <c r="J52" s="91">
-        <f>IF(I52="Líder de proyecto",[5]Recursos!E$5,(IF(I52="Analista",[5]Recursos!E$6,(IF(I52="Diseñador",[5]Recursos!#REF!,(IF(I52="Tester",[5]Recursos!E$7,(IF(I52="Desarrollador",[5]Recursos!E$8,(IF(I52="Arquitecto",[5]Recursos!E$12,(IF(I52="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>31.977576754385964</v>
+        <f>IF(I52="Líder de proyecto",Recursos!E$5,(IF(I52="Analista",Recursos!E$6,(IF(I52="Administrador de la configuración",Recursos!E$11,(IF(I52="Tester",Recursos!E$7,(IF(I52="Desarrollador",Recursos!E$8,(IF(I52="Arquitecto",Recursos!E$12,(IF(I52="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>43.3577850877193</v>
       </c>
       <c r="K52" s="128">
         <f>F52*J52*G52</f>
-        <v>703.50668859649124</v>
+        <v>953.87127192982462</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -6648,12 +6590,12 @@
         <v>85</v>
       </c>
       <c r="J53" s="91">
-        <f>IF(I53="Líder de proyecto",[5]Recursos!E$5,(IF(I53="Analista",[5]Recursos!E$6,(IF(I53="Diseñador",[5]Recursos!#REF!,(IF(I53="Tester",[5]Recursos!E$7,(IF(I53="Desarrollador",[5]Recursos!E$8,(IF(I53="Arquitecto",[5]Recursos!E$12,(IF(I53="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I53="Líder de proyecto",Recursos!E$5,(IF(I53="Analista",Recursos!E$6,(IF(I53="Administrador de la configuración",Recursos!E$11,(IF(I53="Tester",Recursos!E$7,(IF(I53="Desarrollador",Recursos!E$8,(IF(I53="Arquitecto",Recursos!E$12,(IF(I53="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K53" s="128">
         <f>F53*J53*G53</f>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -6679,12 +6621,12 @@
         <v>85</v>
       </c>
       <c r="J54" s="91">
-        <f>IF(I54="Líder de proyecto",[5]Recursos!E$5,(IF(I54="Analista",[5]Recursos!E$6,(IF(I54="Diseñador",[5]Recursos!#REF!,(IF(I54="Tester",[5]Recursos!E$7,(IF(I54="Desarrollador",[5]Recursos!E$8,(IF(I54="Arquitecto",[5]Recursos!E$12,(IF(I54="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
-        <v>59.853275767543863</v>
+        <f>IF(I54="Líder de proyecto",Recursos!E$5,(IF(I54="Analista",Recursos!E$6,(IF(I54="Administrador de la configuración",Recursos!E$11,(IF(I54="Tester",Recursos!E$7,(IF(I54="Desarrollador",Recursos!E$8,(IF(I54="Arquitecto",Recursos!E$12,(IF(I54="Aseguramiento de la calidad",Recursos!E$9,0)))))))))))))</f>
+        <v>71.233484100877192</v>
       </c>
       <c r="K54" s="128">
         <f>F54*J54*G54</f>
-        <v>239.41310307017545</v>
+        <v>284.93393640350877</v>
       </c>
       <c r="L54" s="90"/>
     </row>
@@ -6731,7 +6673,7 @@
       <c r="J56" s="239"/>
       <c r="K56" s="83">
         <f>SUM(K50+K47+K30+K16+K9+K55)</f>
-        <v>12626.448067434212</v>
+        <v>15289.41681743421</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -6744,7 +6686,7 @@
       <c r="J57" s="162"/>
       <c r="K57" s="163">
         <f>(200*F7)-K56</f>
-        <v>32573.551932565788</v>
+        <v>29910.583182565788</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -6882,7 +6824,7 @@
   <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6926,7 +6868,7 @@
       </c>
       <c r="E5" s="85">
         <f t="shared" ref="E5:E12" si="0">SUM(D5+E$27)</f>
-        <v>59.853275767543863</v>
+        <v>71.233484100877192</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -6942,7 +6884,7 @@
       </c>
       <c r="E6" s="85">
         <f t="shared" si="0"/>
-        <v>51.617173793859649</v>
+        <v>62.997382127192978</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -6958,7 +6900,7 @@
       </c>
       <c r="E7" s="85">
         <f t="shared" si="0"/>
-        <v>51.617173793859649</v>
+        <v>62.997382127192978</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -6974,7 +6916,7 @@
       </c>
       <c r="E8" s="85">
         <f t="shared" si="0"/>
-        <v>59.853275767543863</v>
+        <v>71.233484100877192</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -6990,7 +6932,7 @@
       </c>
       <c r="E9" s="85">
         <f t="shared" si="0"/>
-        <v>31.977576754385964</v>
+        <v>43.3577850877193</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
@@ -7006,7 +6948,7 @@
       </c>
       <c r="E10" s="85">
         <f t="shared" si="0"/>
-        <v>49.11236293859649</v>
+        <v>60.492571271929819</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -7022,7 +6964,7 @@
       </c>
       <c r="E11" s="85">
         <f t="shared" si="0"/>
-        <v>31.977576754385964</v>
+        <v>43.3577850877193</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -7038,7 +6980,7 @@
       </c>
       <c r="E12" s="120">
         <f t="shared" si="0"/>
-        <v>59.853275767543863</v>
+        <v>71.233484100877192</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -7121,14 +7063,14 @@
         <v>99</v>
       </c>
       <c r="C27" s="73">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D27" s="167" t="s">
         <v>100</v>
       </c>
       <c r="E27" s="87">
         <f>((C23/C27)/30/8)</f>
-        <v>11.380208333333334</v>
+        <v>22.760416666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>